<commit_message>
check in part list update
</commit_message>
<xml_diff>
--- a/partlist.xlsx
+++ b/partlist.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\pi\eta-3400\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B7FD01F5-12D9-4E9C-AD08-DE939BA084CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF331E08-4167-4A5E-A082-3E10917B8CD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28920" yWindow="2340" windowWidth="28875" windowHeight="19455"/>
+    <workbookView xWindow="28725" yWindow="2340" windowWidth="28875" windowHeight="19455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="partlist" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="119">
   <si>
     <t>Part</t>
   </si>
@@ -265,9 +265,6 @@
     <t>digikey 1N4148FS-ND</t>
   </si>
   <si>
-    <t>digikey 1450-1033-ND</t>
-  </si>
-  <si>
     <t>ebay</t>
   </si>
   <si>
@@ -347,12 +344,45 @@
   </si>
   <si>
     <t>DCJACK 5.5x2.1</t>
+  </si>
+  <si>
+    <t>470uf/16V</t>
+  </si>
+  <si>
+    <t>additional stability when using pi; place across the 5V and GND pins of SV1</t>
+  </si>
+  <si>
+    <t>CAB1</t>
+  </si>
+  <si>
+    <t>40 pin ribbon cable</t>
+  </si>
+  <si>
+    <t>40-ribbon</t>
+  </si>
+  <si>
+    <t>IDC1, IDC2</t>
+  </si>
+  <si>
+    <t>2x20 IDC conn</t>
+  </si>
+  <si>
+    <t>2x20 IDC ribbon cable connector</t>
+  </si>
+  <si>
+    <t>ETA-3400 to ET-3400 cable</t>
+  </si>
+  <si>
+    <t>ETA-3400 to ET-3400 connectors</t>
+  </si>
+  <si>
+    <t>digikey 1450-1182-5-ND (use the 70ns version, not the 55ns)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1190,11 +1220,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,7 +1263,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1247,7 +1277,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1261,7 +1291,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1282,401 +1312,440 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>44</v>
-      </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>108</v>
       </c>
       <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>80</v>
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" t="s">
-        <v>86</v>
+        <v>2</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E8" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
-        <v>82</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>107</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
         <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
         <v>62</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="E20" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="E21" t="s">
-        <v>98</v>
+        <v>62</v>
+      </c>
+      <c r="D21" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23">
         <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C26">
-        <v>7</v>
-      </c>
-      <c r="D26" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>97</v>
+        <v>76</v>
+      </c>
+      <c r="E27" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
         <v>96</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
-        <v>95</v>
-      </c>
-      <c r="E28" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E29" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
+      <c r="D30" t="s">
+        <v>103</v>
+      </c>
       <c r="E30" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>36</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>37</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34" t="s">
         <v>89</v>
       </c>
-      <c r="E33" t="s">
-        <v>90</v>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" t="s">
+        <v>111</v>
+      </c>
+      <c r="F35" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" t="s">
+        <v>115</v>
+      </c>
+      <c r="F36" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add DB25 to BOM
</commit_message>
<xml_diff>
--- a/partlist.xlsx
+++ b/partlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\pi\eta-3400\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF331E08-4167-4A5E-A082-3E10917B8CD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03243B67-0423-4E6F-A216-5651F703B67D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28725" yWindow="2340" windowWidth="28875" windowHeight="19455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22770" yWindow="2130" windowWidth="28875" windowHeight="19455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="partlist" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="123">
   <si>
     <t>Part</t>
   </si>
@@ -377,6 +377,18 @@
   </si>
   <si>
     <t>digikey 1450-1182-5-ND (use the 70ns version, not the 55ns)</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>DB25</t>
+  </si>
+  <si>
+    <t>DB25 connector</t>
+  </si>
+  <si>
+    <t>Digikey, AE10935-ND</t>
   </si>
 </sst>
 </file>
@@ -1221,10 +1233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1713,38 +1725,55 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>119</v>
+      </c>
       <c r="B34" t="s">
+        <v>120</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>121</v>
+      </c>
+      <c r="E34" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>88</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>110</v>
-      </c>
-      <c r="B35" t="s">
-        <v>112</v>
-      </c>
-      <c r="D35" t="s">
-        <v>111</v>
-      </c>
-      <c r="F35" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" t="s">
+        <v>111</v>
+      </c>
+      <c r="F36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>113</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>114</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>115</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F37" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>